<commit_message>
ADD coordinates cleaning function
</commit_message>
<xml_diff>
--- a/fuentes/combinadas/combinadas_v0.9.xlsx
+++ b/fuentes/combinadas/combinadas_v0.9.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="false" showVerticalScroll="false" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ONAMET" sheetId="1" state="visible" r:id="rId2"/>
@@ -4152,7 +4152,7 @@
       <selection pane="topLeft" activeCell="F85" activeCellId="0" sqref="F85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.06"/>
@@ -7412,10 +7412,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -8162,10 +8162,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -8932,10 +8932,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -9568,10 +9568,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -9584,7 +9584,7 @@
   <dimension ref="A1:O176"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10847,7 +10847,7 @@
         <v>2065279</v>
       </c>
       <c r="H29" s="6" t="n">
-        <v>3446360</v>
+        <v>344636</v>
       </c>
       <c r="I29" s="6" t="n">
         <v>2065264</v>
@@ -16764,10 +16764,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -19297,10 +19297,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
UPDATE stations lists INDRHI gauge added
</commit_message>
<xml_diff>
--- a/fuentes/combinadas/combinadas_v0.9.xlsx
+++ b/fuentes/combinadas/combinadas_v0.9.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="false" showVerticalScroll="false" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ONAMET" sheetId="1" state="visible" r:id="rId2"/>
@@ -2081,7 +2081,7 @@
     <t xml:space="preserve">19 16 48</t>
   </si>
   <si>
-    <t xml:space="preserve">59 57 57</t>
+    <t xml:space="preserve">69 57 57</t>
   </si>
   <si>
     <t xml:space="preserve">1980-2018</t>
@@ -4152,7 +4152,7 @@
       <selection pane="topLeft" activeCell="F85" activeCellId="0" sqref="F85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.06"/>
@@ -7412,7 +7412,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -8162,7 +8162,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -8932,7 +8932,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -9568,7 +9568,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -9584,7 +9584,7 @@
   <dimension ref="A1:O176"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
+      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16764,7 +16764,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -19297,7 +19297,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
UPDATE climate stations from INDRHI added
</commit_message>
<xml_diff>
--- a/fuentes/combinadas/combinadas_v0.9.xlsx
+++ b/fuentes/combinadas/combinadas_v0.9.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ONAMET" sheetId="1" state="visible" r:id="rId2"/>
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3129" uniqueCount="1249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3129" uniqueCount="1248">
   <si>
     <t xml:space="preserve">codigo</t>
   </si>
@@ -3842,13 +3842,10 @@
     <t xml:space="preserve">Es una de las mejores estaciones en la región, de las mas estables.</t>
   </si>
   <si>
-    <t xml:space="preserve">estación Vallejuelo</t>
-  </si>
-  <si>
     <t xml:space="preserve">No existe garita y no tiene termómetro.</t>
   </si>
   <si>
-    <t xml:space="preserve">Km 11 Carretera  Sánchez</t>
+    <t xml:space="preserve">Km 11 Carretera Sánchez</t>
   </si>
   <si>
     <t xml:space="preserve">San Juan de la  Maguana</t>
@@ -4152,7 +4149,7 @@
       <selection pane="topLeft" activeCell="F85" activeCellId="0" sqref="F85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.06"/>
@@ -9583,7 +9580,7 @@
   </sheetPr>
   <dimension ref="A1:O176"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
@@ -16779,8 +16776,8 @@
   </sheetPr>
   <dimension ref="A1:O79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18450,7 +18447,7 @@
         <v>47</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>1200</v>
+        <v>841</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>1057</v>
@@ -18471,15 +18468,15 @@
         <v>1069</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="n">
         <v>48</v>
       </c>
-      <c r="C49" s="6" t="s">
-        <v>1202</v>
+      <c r="C49" s="7" t="s">
+        <v>1201</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>1057</v>
@@ -18488,10 +18485,10 @@
         <v>647</v>
       </c>
       <c r="F49" s="6" t="s">
+        <v>1202</v>
+      </c>
+      <c r="G49" s="6" t="s">
         <v>1203</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>1204</v>
       </c>
       <c r="H49" s="6" t="s">
         <v>1067</v>
@@ -18503,7 +18500,7 @@
         <v>1069</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18511,7 +18508,7 @@
         <v>49</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>1057</v>
@@ -18520,7 +18517,7 @@
         <v>1157</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="H50" s="6" t="s">
         <v>1067</v>
@@ -18532,7 +18529,7 @@
         <v>1069</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18540,7 +18537,7 @@
         <v>50</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>1057</v>
@@ -18549,7 +18546,7 @@
         <v>1157</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="H51" s="6" t="s">
         <v>1079</v>
@@ -18558,7 +18555,7 @@
         <v>1080</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18566,7 +18563,7 @@
         <v>51</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>1057</v>
@@ -18575,7 +18572,7 @@
         <v>1057</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>1067</v>
@@ -18587,7 +18584,7 @@
         <v>1069</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18595,13 +18592,13 @@
         <v>52</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>1057</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>1079</v>
@@ -18610,10 +18607,10 @@
         <v>1080</v>
       </c>
       <c r="J53" s="6" t="s">
+        <v>1213</v>
+      </c>
+      <c r="K53" s="6" t="s">
         <v>1214</v>
-      </c>
-      <c r="K53" s="6" t="s">
-        <v>1215</v>
       </c>
       <c r="M53" s="7"/>
       <c r="N53" s="7"/>
@@ -18627,7 +18624,7 @@
         <v>1815</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>906</v>
@@ -18636,10 +18633,10 @@
         <v>906</v>
       </c>
       <c r="F54" s="6" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G54" s="6" t="s">
         <v>1217</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>1218</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>1067</v>
@@ -18651,7 +18648,7 @@
         <v>1069</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="M54" s="7"/>
       <c r="N54" s="7"/>
@@ -18665,7 +18662,7 @@
         <v>1802</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>906</v>
@@ -18674,7 +18671,7 @@
         <v>906</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="G55" s="6" t="s">
         <v>985</v>
@@ -18686,10 +18683,10 @@
         <v>1068</v>
       </c>
       <c r="J55" s="6" t="s">
+        <v>1221</v>
+      </c>
+      <c r="K55" s="6" t="s">
         <v>1222</v>
-      </c>
-      <c r="K55" s="6" t="s">
-        <v>1223</v>
       </c>
       <c r="M55" s="7"/>
       <c r="N55" s="7"/>
@@ -18703,7 +18700,7 @@
         <v>1814</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>906</v>
@@ -18712,7 +18709,7 @@
         <v>906</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="G56" s="6" t="s">
         <v>1041</v>
@@ -18727,7 +18724,7 @@
         <v>1069</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="M56" s="7"/>
       <c r="N56" s="7"/>
@@ -18741,7 +18738,7 @@
         <v>1843</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>906</v>
@@ -18750,7 +18747,7 @@
         <v>906</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>1041</v>
@@ -18765,7 +18762,7 @@
         <v>1069</v>
       </c>
       <c r="K57" s="6" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="M57" s="7"/>
       <c r="N57" s="7"/>
@@ -18779,7 +18776,7 @@
         <v>1817</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>906</v>
@@ -18788,22 +18785,22 @@
         <v>906</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="G58" s="6" t="s">
         <v>985</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="I58" s="6" t="s">
         <v>1080</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="M58" s="7"/>
       <c r="N58" s="7"/>
@@ -18824,7 +18821,7 @@
         <v>930</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="G59" s="7" t="s">
         <v>985</v>
@@ -18836,10 +18833,10 @@
         <v>550</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="K59" s="7" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="L59" s="7"/>
       <c r="M59" s="7"/>
@@ -18854,31 +18851,31 @@
         <v>1838</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>906</v>
       </c>
       <c r="E60" s="7" t="s">
+        <v>1232</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>1224</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>1233</v>
       </c>
-      <c r="F60" s="7" t="s">
-        <v>1225</v>
-      </c>
-      <c r="G60" s="7" t="s">
+      <c r="H60" s="7" t="s">
         <v>1234</v>
-      </c>
-      <c r="H60" s="7" t="s">
-        <v>1235</v>
       </c>
       <c r="I60" s="7" t="s">
         <v>550</v>
       </c>
       <c r="J60" s="7" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="K60" s="7" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="L60" s="7"/>
       <c r="M60" s="7"/>
@@ -18902,7 +18899,7 @@
         <v>906</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="G61" s="7" t="s">
         <v>1149</v>
@@ -18914,10 +18911,10 @@
         <v>550</v>
       </c>
       <c r="J61" s="7" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="K61" s="7" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="L61" s="7"/>
       <c r="M61" s="7"/>
@@ -18932,7 +18929,7 @@
         <v>1816</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>906</v>
@@ -18941,10 +18938,10 @@
         <v>906</v>
       </c>
       <c r="F62" s="7" t="s">
+        <v>1239</v>
+      </c>
+      <c r="G62" s="7" t="s">
         <v>1240</v>
-      </c>
-      <c r="G62" s="7" t="s">
-        <v>1241</v>
       </c>
       <c r="H62" s="7" t="s">
         <v>1079</v>
@@ -18953,10 +18950,10 @@
         <v>550</v>
       </c>
       <c r="J62" s="7" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="K62" s="7" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="L62" s="7"/>
       <c r="M62" s="7"/>
@@ -18971,7 +18968,7 @@
         <v>1806</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>906</v>
@@ -18980,10 +18977,10 @@
         <v>906</v>
       </c>
       <c r="F63" s="7" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G63" s="7" t="s">
         <v>1217</v>
-      </c>
-      <c r="G63" s="7" t="s">
-        <v>1218</v>
       </c>
       <c r="H63" s="7" t="s">
         <v>1079</v>
@@ -18992,10 +18989,10 @@
         <v>550</v>
       </c>
       <c r="J63" s="7" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="K63" s="7" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="L63" s="7"/>
       <c r="M63" s="7"/>
@@ -19008,13 +19005,13 @@
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="7" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D64" s="7" t="s">
         <v>1245</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="E64" s="7" t="s">
         <v>1246</v>
-      </c>
-      <c r="E64" s="7" t="s">
-        <v>1247</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>1173</v>
@@ -19023,16 +19020,16 @@
         <v>1173</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="I64" s="7" t="s">
         <v>1068</v>
       </c>
       <c r="J64" s="7" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="K64" s="7" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="L64" s="7"/>
       <c r="M64" s="7"/>

</xml_diff>